<commit_message>
Marked Transmittal and DOCS suites for execution.
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/suite/Suite.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/suite/Suite.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LeapThoughtProjectWS\FluidTX_Trunk\src\com\proj\suite\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITWS_Fluid_Sprint1\Fulcrum_FluidTX_Trunk\src\com\proj\suite\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -480,9 +480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -551,7 +549,7 @@
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>